<commit_message>
agrego costos y mejor graf BM
</commit_message>
<xml_diff>
--- a/analisis/data/brazil/Grinberg (2021) Renta petrolera Brasil_informePIOYPFConicet.xlsx
+++ b/analisis/data/brazil/Grinberg (2021) Renta petrolera Brasil_informePIOYPFConicet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8719B620-2080-472C-BF41-9BE3E56B9FE1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45297E7-23EB-4321-9966-A5453E547142}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" xr2:uid="{0B5E1281-709A-40E0-9041-0F7FCED6AB17}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0B5E1281-709A-40E0-9041-0F7FCED6AB17}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="39">
   <si>
     <t>Exp</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>plusvalia</t>
+  </si>
+  <si>
+    <t>PBI</t>
   </si>
 </sst>
 </file>
@@ -157,7 +160,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,6 +177,12 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -195,21 +204,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="ANCLAS,REZONES Y SUS PARTES,DE FUNDICION,DE HIERRO O DE ACERO" xfId="2" xr:uid="{9EC3CDCB-45FA-4DC4-AED1-AECE731F81A6}"/>
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 3" xfId="3" xr:uid="{B2C08F57-A551-4A13-8146-F16CB693EACC}"/>
+    <cellStyle name="Normal 8" xfId="4" xr:uid="{5B381C42-F779-44CC-96C4-515D28BD836F}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -521,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E261C2AB-9964-4F19-A1AB-34855E3741C8}">
-  <dimension ref="A2:AX20"/>
+  <dimension ref="A2:AY20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
+      <selection activeCell="AX1" sqref="AX1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -554,10 +567,10 @@
     <col min="42" max="42" width="11.08984375" bestFit="1" customWidth="1"/>
     <col min="43" max="45" width="10.08984375" bestFit="1" customWidth="1"/>
     <col min="46" max="48" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="50" max="51" width="12.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:51" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -690,8 +703,11 @@
       <c r="AX2" t="s">
         <v>37</v>
       </c>
+      <c r="AY2" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>20</v>
       </c>
@@ -824,8 +840,11 @@
       <c r="AX3" t="s">
         <v>25</v>
       </c>
+      <c r="AY3" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1999</v>
       </c>
@@ -878,7 +897,7 @@
         <v>-712.78525105988615</v>
       </c>
       <c r="R4" s="1"/>
-      <c r="S4" s="1">
+      <c r="S4" s="2">
         <v>1999</v>
       </c>
       <c r="T4" s="1"/>
@@ -897,7 +916,7 @@
       <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
       <c r="AI4" s="1"/>
-      <c r="AJ4" s="1">
+      <c r="AJ4" s="2">
         <v>1999</v>
       </c>
       <c r="AK4" s="1">
@@ -927,8 +946,11 @@
       <c r="AX4" s="1">
         <v>568396.73983307672</v>
       </c>
+      <c r="AY4" s="3">
+        <v>1087710.4560539899</v>
+      </c>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2000</v>
       </c>
@@ -981,7 +1003,7 @@
         <v>8096.0959081835481</v>
       </c>
       <c r="R5" s="1"/>
-      <c r="S5" s="1">
+      <c r="S5" s="2">
         <v>2000</v>
       </c>
       <c r="T5" s="1"/>
@@ -1000,7 +1022,7 @@
       <c r="AG5" s="1"/>
       <c r="AH5" s="1"/>
       <c r="AI5" s="1"/>
-      <c r="AJ5" s="1">
+      <c r="AJ5" s="2">
         <v>2000</v>
       </c>
       <c r="AK5" s="1">
@@ -1030,8 +1052,11 @@
       <c r="AX5" s="1">
         <v>618283.56937427563</v>
       </c>
+      <c r="AY5" s="3">
+        <v>1199092.07094021</v>
+      </c>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2001</v>
       </c>
@@ -1084,7 +1109,7 @@
         <v>2196.7504533844954</v>
       </c>
       <c r="R6" s="1"/>
-      <c r="S6" s="1">
+      <c r="S6" s="2">
         <v>2001</v>
       </c>
       <c r="T6" s="1"/>
@@ -1103,7 +1128,7 @@
       <c r="AG6" s="1"/>
       <c r="AH6" s="1"/>
       <c r="AI6" s="1"/>
-      <c r="AJ6" s="1">
+      <c r="AJ6" s="2">
         <v>2001</v>
       </c>
       <c r="AK6" s="1">
@@ -1133,8 +1158,11 @@
       <c r="AX6" s="1">
         <v>692746.23265307408</v>
       </c>
+      <c r="AY6" s="3">
+        <v>1315755.4678309299</v>
+      </c>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2002</v>
       </c>
@@ -1187,7 +1215,7 @@
         <v>3573.4324972246768</v>
       </c>
       <c r="R7" s="1"/>
-      <c r="S7" s="1">
+      <c r="S7" s="2">
         <v>2002</v>
       </c>
       <c r="T7" s="1">
@@ -1236,7 +1264,7 @@
         <v>1671.8032726368015</v>
       </c>
       <c r="AI7" s="1"/>
-      <c r="AJ7" s="1">
+      <c r="AJ7" s="2">
         <v>2002</v>
       </c>
       <c r="AK7" s="1">
@@ -1278,8 +1306,11 @@
       <c r="AX7" s="1">
         <v>794870.60341896769</v>
       </c>
+      <c r="AY7" s="3">
+        <v>1488787.2551583699</v>
+      </c>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2003</v>
       </c>
@@ -1332,7 +1363,7 @@
         <v>11975.351964593916</v>
       </c>
       <c r="R8" s="1"/>
-      <c r="S8" s="1">
+      <c r="S8" s="2">
         <v>2003</v>
       </c>
       <c r="T8" s="1">
@@ -1381,7 +1412,7 @@
         <v>9310.4220918920655</v>
       </c>
       <c r="AI8" s="1"/>
-      <c r="AJ8" s="1">
+      <c r="AJ8" s="2">
         <v>2003</v>
       </c>
       <c r="AK8" s="1">
@@ -1423,8 +1454,11 @@
       <c r="AX8" s="1">
         <v>972867.03042056132</v>
       </c>
+      <c r="AY8" s="3">
+        <v>1717950.39642449</v>
+      </c>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2004</v>
       </c>
@@ -1477,7 +1511,7 @@
         <v>22474.075290876794</v>
       </c>
       <c r="R9" s="1"/>
-      <c r="S9" s="1">
+      <c r="S9" s="2">
         <v>2004</v>
       </c>
       <c r="T9" s="1">
@@ -1526,7 +1560,7 @@
         <v>17651.746067724227</v>
       </c>
       <c r="AI9" s="1"/>
-      <c r="AJ9" s="1">
+      <c r="AJ9" s="2">
         <v>2004</v>
       </c>
       <c r="AK9" s="1">
@@ -1568,8 +1602,11 @@
       <c r="AX9" s="1">
         <v>1140537.274351012</v>
       </c>
+      <c r="AY9" s="3">
+        <v>1957751.2129625699</v>
+      </c>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2005</v>
       </c>
@@ -1622,7 +1659,7 @@
         <v>54484.830329963705</v>
       </c>
       <c r="R10" s="1"/>
-      <c r="S10" s="1">
+      <c r="S10" s="2">
         <v>2005</v>
       </c>
       <c r="T10" s="1">
@@ -1671,7 +1708,7 @@
         <v>42595.21090117182</v>
       </c>
       <c r="AI10" s="1"/>
-      <c r="AJ10" s="1">
+      <c r="AJ10" s="2">
         <v>2005</v>
       </c>
       <c r="AK10" s="1">
@@ -1713,8 +1750,11 @@
       <c r="AX10" s="1">
         <v>1263670.5487010842</v>
       </c>
+      <c r="AY10" s="3">
+        <v>2170584.5034221401</v>
+      </c>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2006</v>
       </c>
@@ -1767,7 +1807,7 @@
         <v>53806.642828767937</v>
       </c>
       <c r="R11" s="1"/>
-      <c r="S11" s="1">
+      <c r="S11" s="2">
         <v>2006</v>
       </c>
       <c r="T11" s="1">
@@ -1816,7 +1856,7 @@
         <v>42769.527485749662</v>
       </c>
       <c r="AI11" s="1"/>
-      <c r="AJ11" s="1">
+      <c r="AJ11" s="2">
         <v>2006</v>
       </c>
       <c r="AK11" s="1">
@@ -1858,8 +1898,11 @@
       <c r="AX11" s="1">
         <v>1414672.6764631313</v>
       </c>
+      <c r="AY11" s="3">
+        <v>2409449.9220720599</v>
+      </c>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2007</v>
       </c>
@@ -1912,7 +1955,7 @@
         <v>103228.49497948255</v>
       </c>
       <c r="R12" s="1"/>
-      <c r="S12" s="1">
+      <c r="S12" s="2">
         <v>2007</v>
       </c>
       <c r="T12" s="1">
@@ -1961,7 +2004,7 @@
         <v>87067.49881670803</v>
       </c>
       <c r="AI12" s="1"/>
-      <c r="AJ12" s="1">
+      <c r="AJ12" s="2">
         <v>2007</v>
       </c>
       <c r="AK12" s="1">
@@ -2003,8 +2046,11 @@
       <c r="AX12" s="1">
         <v>1633205.6699043843</v>
       </c>
+      <c r="AY12" s="3">
+        <v>2720262.9378383202</v>
+      </c>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2008</v>
       </c>
@@ -2057,7 +2103,7 @@
         <v>182761.87557299106</v>
       </c>
       <c r="R13" s="1"/>
-      <c r="S13" s="1">
+      <c r="S13" s="2">
         <v>2008</v>
       </c>
       <c r="T13" s="1">
@@ -2106,7 +2152,7 @@
         <v>158314.64529849184</v>
       </c>
       <c r="AI13" s="1"/>
-      <c r="AJ13" s="1">
+      <c r="AJ13" s="2">
         <v>2008</v>
       </c>
       <c r="AK13" s="1">
@@ -2148,8 +2194,11 @@
       <c r="AX13" s="1">
         <v>1880095.8803957757</v>
       </c>
+      <c r="AY13" s="3">
+        <v>3109803.0890462901</v>
+      </c>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2009</v>
       </c>
@@ -2202,7 +2251,7 @@
         <v>94861.196888049206</v>
       </c>
       <c r="R14" s="1"/>
-      <c r="S14" s="1">
+      <c r="S14" s="2">
         <v>2009</v>
       </c>
       <c r="T14" s="1">
@@ -2251,7 +2300,7 @@
         <v>75943.726940467081</v>
       </c>
       <c r="AI14" s="1"/>
-      <c r="AJ14" s="1">
+      <c r="AJ14" s="2">
         <v>2009</v>
       </c>
       <c r="AK14" s="1">
@@ -2293,8 +2342,11 @@
       <c r="AX14" s="1">
         <v>1983218.1746469371</v>
       </c>
+      <c r="AY14" s="3">
+        <v>3333039.35542242</v>
+      </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2010</v>
       </c>
@@ -2347,7 +2399,7 @@
         <v>189609.16875848192</v>
       </c>
       <c r="R15" s="1"/>
-      <c r="S15" s="1">
+      <c r="S15" s="2">
         <v>2010</v>
       </c>
       <c r="T15" s="1">
@@ -2396,7 +2448,7 @@
         <v>166323.6900734145</v>
       </c>
       <c r="AI15" s="1"/>
-      <c r="AJ15" s="1">
+      <c r="AJ15" s="2">
         <v>2010</v>
       </c>
       <c r="AK15" s="1">
@@ -2438,8 +2490,11 @@
       <c r="AX15" s="1">
         <v>2368513.4648435162</v>
       </c>
+      <c r="AY15" s="3">
+        <v>3885847</v>
+      </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2011</v>
       </c>
@@ -2492,7 +2547,7 @@
         <v>320715.59625318146</v>
       </c>
       <c r="R16" s="1"/>
-      <c r="S16" s="1">
+      <c r="S16" s="2">
         <v>2011</v>
       </c>
       <c r="T16" s="1">
@@ -2541,7 +2596,7 @@
         <v>289967.21813475766</v>
       </c>
       <c r="AI16" s="1"/>
-      <c r="AJ16" s="1">
+      <c r="AJ16" s="2">
         <v>2011</v>
       </c>
       <c r="AK16" s="1">
@@ -2583,8 +2638,11 @@
       <c r="AX16" s="1">
         <v>2679349.3287103372</v>
       </c>
+      <c r="AY16" s="3">
+        <v>4376382</v>
+      </c>
     </row>
-    <row r="17" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2012</v>
       </c>
@@ -2637,7 +2695,7 @@
         <v>356283.80545998394</v>
       </c>
       <c r="R17" s="1"/>
-      <c r="S17" s="1">
+      <c r="S17" s="2">
         <v>2012</v>
       </c>
       <c r="T17" s="1">
@@ -2686,7 +2744,7 @@
         <v>322839.77534215042</v>
       </c>
       <c r="AI17" s="1"/>
-      <c r="AJ17" s="1">
+      <c r="AJ17" s="2">
         <v>2012</v>
       </c>
       <c r="AK17" s="1">
@@ -2728,8 +2786,11 @@
       <c r="AX17" s="1">
         <v>2943570.9288324099</v>
       </c>
+      <c r="AY17" s="3">
+        <v>4814760</v>
+      </c>
     </row>
-    <row r="18" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2013</v>
       </c>
@@ -2782,7 +2843,7 @@
         <v>346043.37435935094</v>
       </c>
       <c r="R18" s="1"/>
-      <c r="S18" s="1">
+      <c r="S18" s="2">
         <v>2013</v>
       </c>
       <c r="T18" s="1">
@@ -2831,7 +2892,7 @@
         <v>311276.11030317849</v>
       </c>
       <c r="AI18" s="1"/>
-      <c r="AJ18" s="1">
+      <c r="AJ18" s="2">
         <v>2013</v>
       </c>
       <c r="AK18" s="1">
@@ -2873,8 +2934,11 @@
       <c r="AX18" s="1">
         <v>3327043.745585816</v>
       </c>
+      <c r="AY18" s="3">
+        <v>5331619</v>
+      </c>
     </row>
-    <row r="19" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2014</v>
       </c>
@@ -2927,7 +2991,7 @@
         <v>349384.09417433705</v>
       </c>
       <c r="R19" s="1"/>
-      <c r="S19" s="1">
+      <c r="S19" s="2">
         <v>2014</v>
       </c>
       <c r="T19" s="1">
@@ -2976,7 +3040,7 @@
         <v>287318.73065278126</v>
       </c>
       <c r="AI19" s="1"/>
-      <c r="AJ19" s="1">
+      <c r="AJ19" s="2">
         <v>2014</v>
       </c>
       <c r="AK19" s="1">
@@ -3018,8 +3082,11 @@
       <c r="AX19" s="1">
         <v>3547027.4869568069</v>
       </c>
+      <c r="AY19" s="3">
+        <v>5778953</v>
+      </c>
     </row>
-    <row r="20" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2015</v>
       </c>
@@ -3054,25 +3121,25 @@
         <v>10127.019742280954</v>
       </c>
       <c r="L20" s="1">
-        <v>0</v>
+        <v>543311.10811666609</v>
       </c>
       <c r="M20" s="1">
-        <v>10127.019742280954</v>
+        <v>553438.12785894703</v>
       </c>
       <c r="N20" s="1">
-        <v>1089.4619753375844</v>
+        <v>59538.720309489378</v>
       </c>
       <c r="O20" s="1">
-        <v>57.94895574378215</v>
+        <v>112.71026436304093</v>
       </c>
       <c r="P20" s="1">
-        <v>229.48554440549441</v>
+        <v>174.72423578623562</v>
       </c>
       <c r="Q20" s="1">
-        <v>244940.45535268579</v>
+        <v>186491.197018534</v>
       </c>
       <c r="R20" s="1"/>
-      <c r="S20" s="1">
+      <c r="S20" s="2">
         <v>2015</v>
       </c>
       <c r="T20" s="1">
@@ -3103,25 +3170,25 @@
         <v>12669.051488639167</v>
       </c>
       <c r="AC20" s="1">
-        <v>0</v>
+        <v>488979.99730499944</v>
       </c>
       <c r="AD20" s="1">
-        <v>12669.051488639167</v>
+        <v>501649.04879363859</v>
       </c>
       <c r="AE20" s="1">
-        <v>1362.9330456264718</v>
+        <v>53967.26554636308</v>
       </c>
       <c r="AF20" s="1">
-        <v>88.848467633640851</v>
+        <v>149.25142610226101</v>
       </c>
       <c r="AG20" s="1">
-        <v>198.58603251563574</v>
+        <v>138.18307404701557</v>
       </c>
       <c r="AH20" s="1">
-        <v>211959.98796819418</v>
+        <v>147489.13778771125</v>
       </c>
       <c r="AI20" s="1"/>
-      <c r="AJ20" s="1">
+      <c r="AJ20" s="2">
         <v>2015</v>
       </c>
       <c r="AK20" s="1">
@@ -3149,19 +3216,22 @@
         <v>-9729.6927080421192</v>
       </c>
       <c r="AS20" s="1">
-        <v>-10819.154683379704</v>
+        <v>-69268.413017531493</v>
       </c>
       <c r="AT20" s="1">
-        <v>153710.86718447984</v>
+        <v>95261.608850328033</v>
       </c>
       <c r="AU20" s="1">
-        <v>244940.45535268579</v>
+        <v>186491.197018534</v>
       </c>
       <c r="AV20" s="1">
-        <v>211959.98796819418</v>
+        <v>147489.13778771125</v>
       </c>
       <c r="AX20" s="1">
         <v>3688970.1407758752</v>
+      </c>
+      <c r="AY20" s="3">
+        <v>5995787</v>
       </c>
     </row>
   </sheetData>

</xml_diff>